<commit_message>
Adding more otimizations and calculations.
</commit_message>
<xml_diff>
--- a/HarrisCornerDetection/Reports/Board/Timestamps.xlsx
+++ b/HarrisCornerDetection/Reports/Board/Timestamps.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
     <sheet name="Optimized1" sheetId="1" r:id="rId2"/>
     <sheet name="Optimized2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -86,16 +86,40 @@
     <t>_OPTIMIZATION_GET_CONVOLUTION_000_010_021</t>
   </si>
   <si>
-    <t>Performance</t>
-  </si>
-  <si>
-    <t>Perfomance</t>
-  </si>
-  <si>
     <t>Optimized 1</t>
   </si>
   <si>
     <t>OrderStatisticFiltering</t>
+  </si>
+  <si>
+    <t>Performance Gain</t>
+  </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_ORDER_STATISTIC_FILTERING_SPECIALIZED_001</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_ORDER_STATISTIC_FILTERING_SPECIALIZED_000</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_CONVOLUTION_022</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_CONVOLUTION_001</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_CONVOLUTION_002</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_CONVOLUTION_00X_010_02X</t>
+  </si>
+  <si>
+    <t>_OPTIMIZATION_CONVOLUTION_00X_010_02X_GET</t>
   </si>
 </sst>
 </file>
@@ -139,10 +163,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -237,6 +262,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -272,6 +314,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -493,7 +552,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D4">
         <v>50700022</v>
@@ -604,10 +663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H26"/>
+  <dimension ref="B2:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,9 +676,10 @@
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -641,10 +701,13 @@
       <c r="H2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -667,10 +730,14 @@
         <f>D3/$D$3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>(Original!D3-D3)/Original!D3</f>
+        <v>0.47784859979008004</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -693,10 +760,14 @@
         <f>D4/$D$3</f>
         <v>0.12769369483060217</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f>(Original!D4-D4)/Original!D4</f>
+        <v>0.88001366153253346</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -720,7 +791,7 @@
         <v>0.82911367375497436</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -729,7 +800,7 @@
         <v>0.95680736858557647</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -749,10 +820,10 @@
         <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>12</v>
       </c>
@@ -766,19 +837,19 @@
         <v>4672750</v>
       </c>
       <c r="F9">
-        <f>E9/10^3</f>
+        <f t="shared" ref="F9:F16" si="0">E9/10^3</f>
         <v>4672.75</v>
       </c>
       <c r="G9">
-        <f>E9/10^6</f>
+        <f t="shared" ref="G9:G16" si="1">E9/10^6</f>
         <v>4.6727499999999997</v>
       </c>
-      <c r="H9" s="1">
-        <f>($D$5-D9)/$D$5</f>
-        <v>1.3666470028085114E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="3">
+        <f t="shared" ref="H9:H15" si="2">($D$5/$D9)</f>
+        <v>1.013855830317838</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>13</v>
       </c>
@@ -792,19 +863,19 @@
         <v>4487775</v>
       </c>
       <c r="F10">
-        <f>E10/10^3</f>
+        <f t="shared" si="0"/>
         <v>4487.7749999999996</v>
       </c>
       <c r="G10">
-        <f>E10/10^6</f>
+        <f t="shared" si="1"/>
         <v>4.4877750000000001</v>
       </c>
-      <c r="H10" s="1">
-        <f>($D$5-D10)/$D$5</f>
-        <v>5.271126678817397E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H10" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0556443510200464</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -818,19 +889,19 @@
         <v>5508284.5</v>
       </c>
       <c r="F11">
-        <f>E11/10^3</f>
+        <f t="shared" si="0"/>
         <v>5508.2844999999998</v>
       </c>
       <c r="G11">
-        <f>E11/10^6</f>
+        <f t="shared" si="1"/>
         <v>5.5082845000000002</v>
       </c>
-      <c r="H11" s="1">
-        <f>($D$5-D11)/$D$5</f>
-        <v>-0.16269990671376575</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.86006715423791691</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>15</v>
       </c>
@@ -844,19 +915,19 @@
         <v>4602908</v>
       </c>
       <c r="F12">
-        <f>E12/10^3</f>
+        <f t="shared" si="0"/>
         <v>4602.9080000000004</v>
       </c>
       <c r="G12">
-        <f>E12/10^6</f>
+        <f t="shared" si="1"/>
         <v>4.6029080000000002</v>
       </c>
-      <c r="H12" s="1">
-        <f>($D$5-D12)/$D$5</f>
-        <v>2.8408869815258725E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H12" s="3">
+        <f t="shared" si="2"/>
+        <v>1.0292395318696013</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -870,19 +941,19 @@
         <v>1494246.875</v>
       </c>
       <c r="F13">
-        <f>E13/10^3</f>
+        <f t="shared" si="0"/>
         <v>1494.246875</v>
       </c>
       <c r="G13">
-        <f>E13/10^6</f>
+        <f t="shared" si="1"/>
         <v>1.494246875</v>
       </c>
-      <c r="H13" s="1">
-        <f>($D$5-D13)/$D$5</f>
-        <v>0.68459133543116601</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1704899463272747</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -896,19 +967,19 @@
         <v>1324022.375</v>
       </c>
       <c r="F14">
-        <f>E14/10^3</f>
+        <f t="shared" si="0"/>
         <v>1324.022375</v>
       </c>
       <c r="G14">
-        <f>E14/10^6</f>
+        <f t="shared" si="1"/>
         <v>1.324022375</v>
       </c>
-      <c r="H14" s="1">
-        <f>($D$5-D14)/$D$5</f>
-        <v>0.72052265000755333</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5781074925285603</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>18</v>
       </c>
@@ -922,19 +993,19 @@
         <v>1228013.375</v>
       </c>
       <c r="F15">
-        <f>E15/10^3</f>
+        <f t="shared" si="0"/>
         <v>1228.013375</v>
       </c>
       <c r="G15">
-        <f>E15/10^6</f>
+        <f t="shared" si="1"/>
         <v>1.228013375</v>
       </c>
-      <c r="H15" s="1">
-        <f>($D$5-D15)/$D$5</f>
-        <v>0.74078844957073575</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H15" s="3">
+        <f t="shared" si="2"/>
+        <v>3.857852778334768</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>18</v>
       </c>
@@ -948,16 +1019,16 @@
         <v>2203241.75</v>
       </c>
       <c r="F16">
-        <f>E16/10^3</f>
+        <f t="shared" si="0"/>
         <v>2203.2417500000001</v>
       </c>
       <c r="G16">
-        <f>E16/10^6</f>
+        <f t="shared" si="1"/>
         <v>2.2032417500000001</v>
       </c>
-      <c r="H16" s="1">
-        <f>($D$3-D16)/$D$3</f>
-        <v>0.61440847582639935</v>
+      <c r="H16" s="3">
+        <f>($D$3/$D16)</f>
+        <v>2.5934180014542565</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -980,7 +1051,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1004,9 +1075,9 @@
         <f>E19/10^6</f>
         <v>2.4849562500000002</v>
       </c>
-      <c r="H19" s="1">
-        <f>($D$3-D19)/$D$3</f>
-        <v>0.56510533132946528</v>
+      <c r="H19" s="3">
+        <f>($D$3/$D19)</f>
+        <v>2.29940735547985</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1030,9 +1101,9 @@
         <f>E20/10^6</f>
         <v>1.5131645</v>
       </c>
-      <c r="H20" s="1">
-        <f>($D$5-D20)/$D$5</f>
-        <v>0.6805981569949574</v>
+      <c r="H20" s="3">
+        <f>($D$5/$D20)</f>
+        <v>3.1308523162911506</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1060,22 +1131,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H26"/>
+  <dimension ref="B2:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="14.140625" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1098,7 +1169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>20</v>
       </c>
@@ -1124,7 +1195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>20</v>
       </c>
@@ -1150,7 +1221,7 @@
         <v>0.32667673668405772</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -1175,8 +1246,12 @@
         <f>D5/$D$3</f>
         <v>0.50730908673942499</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3">
+        <f>(Optimized1!$D$5/$D5)</f>
+        <v>4.245282629511455</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>11</v>
       </c>
@@ -1185,52 +1260,163 @@
         <v>0.83398582342348271</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>25</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H26" s="1"/>
     </row>
   </sheetData>

</xml_diff>